<commit_message>
adiciona NOME_PROGRAMA ao programa 148
</commit_message>
<xml_diff>
--- a/data-raw/base_qdd_fiscal_fonte_95.xlsx
+++ b/data-raw/base_qdd_fiscal_fonte_95.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fjunior/Projects/splor/dados-qdd-fonte-95/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7C72F30-1203-FA4A-86DF-5D1C8B18CF59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4DF9C29-26D4-5E49-BA87-054A4932A6C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{7E98796A-B986-48F4-8571-13483804D4C3}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="328" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="329" uniqueCount="121">
   <si>
     <t>ANO</t>
   </si>
@@ -1053,7 +1053,7 @@
   <dimension ref="A1:AE39"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="V21" sqref="V21"/>
+      <selection activeCell="AA32" sqref="AA32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4090,7 +4090,9 @@
       <c r="Z32" s="7" t="s">
         <v>96</v>
       </c>
-      <c r="AA32" s="8"/>
+      <c r="AA32" s="8" t="s">
+        <v>97</v>
+      </c>
       <c r="AB32" s="17" t="s">
         <v>34</v>
       </c>

</xml_diff>

<commit_message>
altera elemento CBMMG de 39 para 52 na acao 4120
</commit_message>
<xml_diff>
--- a/data-raw/base_qdd_fiscal_fonte_95.xlsx
+++ b/data-raw/base_qdd_fiscal_fonte_95.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fjunior/Projects/splor/dados-qdd-fonte-95/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4DF9C29-26D4-5E49-BA87-054A4932A6C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7D47B03-2FB2-B948-B9B6-079AFE58CF46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{7E98796A-B986-48F4-8571-13483804D4C3}"/>
   </bookViews>
@@ -1053,7 +1053,7 @@
   <dimension ref="A1:AE39"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="AA32" sqref="AA32"/>
+      <selection activeCell="K27" sqref="K27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3568,7 +3568,7 @@
         <v>90</v>
       </c>
       <c r="K27" s="5">
-        <v>39</v>
+        <v>52</v>
       </c>
       <c r="L27" s="5">
         <v>95</v>

</xml_diff>